<commit_message>
Nogle Chancekort funktioner er implementeret
</commit_message>
<xml_diff>
--- a/CDIO3 Chancekort.xlsx
+++ b/CDIO3 Chancekort.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsr_0\Dropbox\Documents\DTU\Programmering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsr_0\IdeaProjects\CDIOdel3Gruppe1.java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AA6FCD-ED7C-4C4F-B3EA-A8DC7AC02094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C981FEB-AAD0-468D-8D0D-13CE85D7597D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChanceKort" sheetId="1" r:id="rId1"/>
@@ -78,9 +78,6 @@
     <t>?</t>
   </si>
   <si>
-    <t>Giv dette kort til skibet og tag et chancekort mere. Skib: På den næste skal du sejle frem til hvilket som helst ledigt felt og købe det. Hvis der ikke er nogen ledige felter, skal du købe et af en anden spiller.</t>
-  </si>
-  <si>
     <t>Du har spist for meget slik. Betal M2 til banken.</t>
   </si>
   <si>
@@ -99,12 +96,6 @@
     <t>Hunden</t>
   </si>
   <si>
-    <t>Giv dette kort til Hunden og tag et chancekort mere. Hund: På den næste skal du sejle frem til hvilket som helst ledigt felt og købe det. Hvis der ikke er nogen ledige felter, skal du købe et af en anden spiller.</t>
-  </si>
-  <si>
-    <t>Giv dette kort til Katten og tag et chancekort mere. Kat: På den næste skal du sejle frem til hvilket som helst ledigt felt og købe det. Hvis der ikke er nogen ledige felter, skal du købe et af en anden spiller.</t>
-  </si>
-  <si>
     <t>Det er din fødselsdag. Alle giver dig 1 M. Tillyke med fødselsdagen</t>
   </si>
   <si>
@@ -129,9 +120,6 @@
     <t>pengetransaktion med de andre deltagere</t>
   </si>
   <si>
-    <t>Bil: På din næste tur skal du drøne frem til et hvilket som helst ledigt felt og købe det. Hvis det ikke er nogen ledige felter skal du købe et fra en anden spiller!</t>
-  </si>
-  <si>
     <t>Kortet skal overdrages til anden spiller. Denne kan vælg et hvilket som helst felt. Hvis ikke ledigt felt hvordan besluttes hvilket felt der købes?</t>
   </si>
   <si>
@@ -271,6 +259,18 @@
   </si>
   <si>
     <t>ChanceAmnistiFeng</t>
+  </si>
+  <si>
+    <t>Dette chance kort er givet til Bilen. Tag et chancekort mere. Bil: På din næste tur skal du drøne frem til et hvilket som helst ledigt felt og købe det. Hvis det ikke er nogen ledige felter skal du købe et fra en anden spiller!</t>
+  </si>
+  <si>
+    <t>Dette kort er givet til skibet.Tag et chancekort mere. Skib: På den næste skal du sejle frem til hvilket som helst ledigt felt og købe det. Hvis der ikke er nogen ledige felter, skal du købe et af en anden spiller.</t>
+  </si>
+  <si>
+    <t>Dette kort er givet til Katten . Tag et chancekort mere. Kat: På den næste skal du sejle frem til hvilket som helst ledigt felt og købe det. Hvis der ikke er nogen ledige felter, skal du købe et af en anden spiller.</t>
+  </si>
+  <si>
+    <t>Dette kort er givet til Hunden. Tag et chancekort mere. Hund: På den næste skal du sejle frem til hvilket som helst ledigt felt og købe det. Hvis der ikke er nogen ledige felter, skal du købe et af en anden spiller.</t>
   </si>
 </sst>
 </file>
@@ -627,22 +627,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="77.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="31.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="77.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -653,16 +653,16 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -670,22 +670,22 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -696,16 +696,16 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -713,22 +713,22 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -736,19 +736,19 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -756,22 +756,22 @@
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -779,36 +779,36 @@
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -816,22 +816,22 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -839,125 +839,125 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="1" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="E12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>17</v>
-      </c>
-      <c r="E12" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>18</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>19</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -965,56 +965,56 @@
         <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E17" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" t="s">
-        <v>64</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="G18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1022,19 +1022,19 @@
         <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1042,22 +1042,22 @@
         <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1065,19 +1065,19 @@
         <v>6</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G21" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1094,46 +1094,46 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1141,52 +1141,52 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nogle flere Chancekort funktioner er implementeret
</commit_message>
<xml_diff>
--- a/CDIO3 Chancekort.xlsx
+++ b/CDIO3 Chancekort.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsr_0\IdeaProjects\CDIOdel3Gruppe1.java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C981FEB-AAD0-468D-8D0D-13CE85D7597D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DE19F6-156E-44F3-94A4-21F80BF1DA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,9 +60,6 @@
     <t>Nej</t>
   </si>
   <si>
-    <t>Ryk frem til start.</t>
-  </si>
-  <si>
     <t>Konsekvens ikke veldefineret. Spilleren  kan antagelig vælge.</t>
   </si>
   <si>
@@ -81,15 +78,9 @@
     <t>Du har spist for meget slik. Betal M2 til banken.</t>
   </si>
   <si>
-    <t>Du løslades uden omkostninger. Behold dette kort til du får brug for det.</t>
-  </si>
-  <si>
     <t>Spilleren beholder kortet</t>
   </si>
   <si>
-    <t>Ryk frem til Strandpromenaden.</t>
-  </si>
-  <si>
     <t>Katten</t>
   </si>
   <si>
@@ -141,9 +132,6 @@
     <t>Gratis felt. Ryk frem til et rødt felt. Hvis det der ledigt, får du det gratis. Ellers skal du betale leje ejeren.</t>
   </si>
   <si>
-    <t>Gratis felt. Ryk frem til Skaterparken for at lave det perfekte grind. Hvis ingen ejer den, får du den gratis. Ellers skal du betale leje ejeren.</t>
-  </si>
-  <si>
     <t>Gratis felt. Ryk frem til et lyseblåt eller rødt felt. Hvis det der ledigt, får du det gratis. Ellers skal du betale leje ejeren.</t>
   </si>
   <si>
@@ -271,6 +259,18 @@
   </si>
   <si>
     <t>Dette kort er givet til Hunden. Tag et chancekort mere. Hund: På den næste skal du sejle frem til hvilket som helst ledigt felt og købe det. Hvis der ikke er nogen ledige felter, skal du købe et af en anden spiller.</t>
+  </si>
+  <si>
+    <t>Du løslades uden omkostninger. Du har nu dette indtil du får brug for det.</t>
+  </si>
+  <si>
+    <t>Du rykkes frem til start.</t>
+  </si>
+  <si>
+    <t>Du rykkes frem til Strandpromenaden.</t>
+  </si>
+  <si>
+    <t>Gratis felt. Du kykkes frem til Skaterparken for at lave det perfekte grind. Hvis ingen ejer den, får du den gratis. Ellers skal du betale leje ejeren.</t>
   </si>
 </sst>
 </file>
@@ -627,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -653,13 +653,13 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -670,19 +670,19 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -693,16 +693,16 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -713,19 +713,19 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -736,16 +736,16 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -753,59 +753,59 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -816,19 +816,19 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -839,16 +839,16 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -859,16 +859,16 @@
         <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -879,62 +879,62 @@
         <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -945,16 +945,16 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G15" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -965,33 +965,33 @@
         <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C17" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E17" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G17" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1002,16 +1002,16 @@
         <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G18" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1022,16 +1022,16 @@
         <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1042,19 +1042,19 @@
         <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G20" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1065,19 +1065,19 @@
         <v>6</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G21" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1098,15 +1098,15 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1114,7 +1114,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1122,7 +1122,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1130,7 +1130,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1138,7 +1138,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1146,7 +1146,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1154,7 +1154,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1162,7 +1162,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1170,7 +1170,7 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1178,7 +1178,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1186,7 +1186,7 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Chance et niveau op.
</commit_message>
<xml_diff>
--- a/CDIO3 Chancekort.xlsx
+++ b/CDIO3 Chancekort.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsr_0\IdeaProjects\CDIOdel3Gruppe1.java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DE19F6-156E-44F3-94A4-21F80BF1DA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96A1A29-7993-48C3-805C-E6AF3B2D0BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -628,7 +628,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>